<commit_message>
Test de aitken converge mais plus d'itération
</commit_message>
<xml_diff>
--- a/code-Noé/pagerank/TD2_resultat.xlsx
+++ b/code-Noé/pagerank/TD2_resultat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\documents\Master\AMIS\cours\M1\S2\MIN17211_Méthodes_de_Ranking\Projet\Projet-Ranking-Sujet-11\code-Noé\pagerank\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAC855D-9742-40BF-9780-FE09029064A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3F9267-1145-4F0A-AF2F-8D83CA27DDD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{F232B7C4-8761-42C5-9DC9-0B87264A3A5D}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="20376" windowHeight="9420" activeTab="1" xr2:uid="{F232B7C4-8761-42C5-9DC9-0B87264A3A5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -145,27 +145,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -495,26 +491,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="K2" s="6" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="K2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
@@ -830,26 +826,26 @@
       <c r="R9" s="4"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="K11" s="6" t="s">
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="K11" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
@@ -1118,26 +1114,26 @@
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="K20" s="6" t="s">
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="K20" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="6"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
@@ -1424,8 +1420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3141B3-E7D1-4801-9B2A-1921A6AC73B0}">
   <dimension ref="A1:W53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R44" sqref="R44"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1448,127 +1444,117 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="9">
         <v>1E-3</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9">
         <v>1E-4</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8">
+      <c r="E2" s="9"/>
+      <c r="F2" s="9">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8">
+      <c r="G2" s="9"/>
+      <c r="H2" s="9">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8">
+      <c r="I2" s="9"/>
+      <c r="J2" s="9">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8">
+      <c r="K2" s="9"/>
+      <c r="L2" s="9">
         <v>1E-8</v>
       </c>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8">
+      <c r="M2" s="9"/>
+      <c r="N2" s="9">
         <v>1.0000000000000001E-9</v>
       </c>
-      <c r="O2" s="8"/>
+      <c r="O2" s="9"/>
       <c r="P2" s="1"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="11"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="O3" s="7" t="s">
+      <c r="B3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3" s="6" t="s">
         <v>16</v>
       </c>
       <c r="P3" s="1"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
-      <c r="W3" s="11"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
@@ -1577,7 +1563,7 @@
       <c r="B4" s="2">
         <v>7</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="2">
         <v>2654</v>
       </c>
       <c r="D4" s="2">
@@ -1616,13 +1602,6 @@
       <c r="O4" s="2">
         <v>8259</v>
       </c>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
@@ -1670,13 +1649,6 @@
       <c r="O5" s="2">
         <v>15895</v>
       </c>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
-      <c r="V5" s="10"/>
-      <c r="W5" s="10"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
@@ -1724,13 +1696,6 @@
       <c r="O6" s="2">
         <v>31474</v>
       </c>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="10"/>
-      <c r="W6" s="10"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
@@ -1778,13 +1743,6 @@
       <c r="O7" s="2">
         <v>51555</v>
       </c>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
-      <c r="U7" s="10"/>
-      <c r="V7" s="10"/>
-      <c r="W7" s="10"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
@@ -1832,110 +1790,103 @@
       <c r="O8" s="2">
         <v>423682</v>
       </c>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
-      <c r="V8" s="10"/>
-      <c r="W8" s="10"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="9">
         <v>1E-3</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8">
+      <c r="C11" s="9"/>
+      <c r="D11" s="9">
         <v>1E-4</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8">
+      <c r="E11" s="9"/>
+      <c r="F11" s="9">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8">
+      <c r="G11" s="9"/>
+      <c r="H11" s="9">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8">
+      <c r="I11" s="9"/>
+      <c r="J11" s="9">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8">
+      <c r="K11" s="9"/>
+      <c r="L11" s="9">
         <v>1E-8</v>
       </c>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8">
+      <c r="M11" s="9"/>
+      <c r="N11" s="9">
         <v>1.0000000000000001E-9</v>
       </c>
-      <c r="O11" s="8"/>
+      <c r="O11" s="9"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="M12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N12" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="O12" s="7" t="s">
+      <c r="B12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="O12" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2175,101 +2126,101 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="9">
         <v>1E-3</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8">
+      <c r="C20" s="9"/>
+      <c r="D20" s="9">
         <v>1E-4</v>
       </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8">
+      <c r="E20" s="9"/>
+      <c r="F20" s="9">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8">
+      <c r="G20" s="9"/>
+      <c r="H20" s="9">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8">
+      <c r="I20" s="9"/>
+      <c r="J20" s="9">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8">
+      <c r="K20" s="9"/>
+      <c r="L20" s="9">
         <v>1E-8</v>
       </c>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8">
+      <c r="M20" s="9"/>
+      <c r="N20" s="9">
         <v>1.0000000000000001E-9</v>
       </c>
-      <c r="O20" s="8"/>
+      <c r="O20" s="9"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J21" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="L21" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="M21" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N21" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="O21" s="7" t="s">
+      <c r="B21" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="O21" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2509,101 +2460,101 @@
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="13"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="8">
+      <c r="B29" s="9">
         <v>1E-3</v>
       </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8">
+      <c r="C29" s="9"/>
+      <c r="D29" s="9">
         <v>1E-4</v>
       </c>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8">
+      <c r="E29" s="9"/>
+      <c r="F29" s="9">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8">
+      <c r="G29" s="9"/>
+      <c r="H29" s="9">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8">
+      <c r="I29" s="9"/>
+      <c r="J29" s="9">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8">
+      <c r="K29" s="9"/>
+      <c r="L29" s="9">
         <v>1E-8</v>
       </c>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8">
+      <c r="M29" s="9"/>
+      <c r="N29" s="9">
         <v>1.0000000000000001E-9</v>
       </c>
-      <c r="O29" s="8"/>
+      <c r="O29" s="9"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I30" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J30" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="K30" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="L30" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="M30" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N30" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="O30" s="7" t="s">
+      <c r="B30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M30" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="O30" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2843,101 +2794,101 @@
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A37" s="13" t="s">
+      <c r="A37" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="13"/>
-      <c r="M37" s="13"/>
-      <c r="N37" s="13"/>
-      <c r="O37" s="13"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B38" s="8">
+      <c r="B38" s="9">
         <v>1E-3</v>
       </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8">
+      <c r="C38" s="9"/>
+      <c r="D38" s="9">
         <v>1E-4</v>
       </c>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8">
+      <c r="E38" s="9"/>
+      <c r="F38" s="9">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8">
+      <c r="G38" s="9"/>
+      <c r="H38" s="9">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8">
+      <c r="I38" s="9"/>
+      <c r="J38" s="9">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8">
+      <c r="K38" s="9"/>
+      <c r="L38" s="9">
         <v>1E-8</v>
       </c>
-      <c r="M38" s="8"/>
-      <c r="N38" s="8">
+      <c r="M38" s="9"/>
+      <c r="N38" s="9">
         <v>1.0000000000000001E-9</v>
       </c>
-      <c r="O38" s="8"/>
+      <c r="O38" s="9"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B39" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H39" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I39" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J39" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="K39" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="L39" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="M39" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N39" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="O39" s="7" t="s">
+      <c r="B39" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J39" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L39" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M39" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N39" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="O39" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -3177,101 +3128,101 @@
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A46" s="13" t="s">
+      <c r="A46" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B46" s="13"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="13"/>
-      <c r="I46" s="13"/>
-      <c r="J46" s="13"/>
-      <c r="K46" s="13"/>
-      <c r="L46" s="13"/>
-      <c r="M46" s="13"/>
-      <c r="N46" s="13"/>
-      <c r="O46" s="13"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="8"/>
+      <c r="M46" s="8"/>
+      <c r="N46" s="8"/>
+      <c r="O46" s="8"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B47" s="8">
+      <c r="B47" s="9">
         <v>1E-3</v>
       </c>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8">
+      <c r="C47" s="9"/>
+      <c r="D47" s="9">
         <v>1E-4</v>
       </c>
-      <c r="E47" s="8"/>
-      <c r="F47" s="8">
+      <c r="E47" s="9"/>
+      <c r="F47" s="9">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8">
+      <c r="G47" s="9"/>
+      <c r="H47" s="9">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="I47" s="8"/>
-      <c r="J47" s="8">
+      <c r="I47" s="9"/>
+      <c r="J47" s="9">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="K47" s="8"/>
-      <c r="L47" s="8">
+      <c r="K47" s="9"/>
+      <c r="L47" s="9">
         <v>1E-8</v>
       </c>
-      <c r="M47" s="8"/>
-      <c r="N47" s="8">
+      <c r="M47" s="9"/>
+      <c r="N47" s="9">
         <v>1.0000000000000001E-9</v>
       </c>
-      <c r="O47" s="8"/>
+      <c r="O47" s="9"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B48" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G48" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H48" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I48" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J48" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="K48" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="L48" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="M48" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N48" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="O48" s="7" t="s">
+      <c r="B48" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H48" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I48" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J48" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K48" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L48" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M48" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N48" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="O48" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -3372,30 +3323,15 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="A46:O46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="L47:M47"/>
-    <mergeCell ref="N47:O47"/>
-    <mergeCell ref="A37:O37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="L38:M38"/>
-    <mergeCell ref="N38:O38"/>
-    <mergeCell ref="A28:O28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A10:O10"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
     <mergeCell ref="N11:O11"/>
     <mergeCell ref="A19:O19"/>
     <mergeCell ref="B20:C20"/>
@@ -3411,15 +3347,30 @@
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="L11:M11"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A10:O10"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A28:O28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="A37:O37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="L38:M38"/>
+    <mergeCell ref="N38:O38"/>
+    <mergeCell ref="A46:O46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="L47:M47"/>
+    <mergeCell ref="N47:O47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
tous les fichiers fait avec pagerank
</commit_message>
<xml_diff>
--- a/code-Noé/pagerank/TD2_resultat.xlsx
+++ b/code-Noé/pagerank/TD2_resultat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\documents\Master\AMIS\cours\M1\S2\MIN17211_Méthodes_de_Ranking\Projet\Projet-Ranking-Sujet-11\code-Noé\pagerank\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3F9267-1145-4F0A-AF2F-8D83CA27DDD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081357DE-2B81-4C12-8FC4-96C0CD01F213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="20376" windowHeight="9420" activeTab="1" xr2:uid="{F232B7C4-8761-42C5-9DC9-0B87264A3A5D}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13056" activeTab="1" xr2:uid="{F232B7C4-8761-42C5-9DC9-0B87264A3A5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -158,10 +158,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -480,7 +480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B67617D-60B1-476F-9C73-7EB7FC7C251C}">
   <dimension ref="B2:R27"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="R13" sqref="R13:R17"/>
     </sheetView>
   </sheetViews>
@@ -1420,8 +1420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3141B3-E7D1-4801-9B2A-1921A6AC73B0}">
   <dimension ref="A1:W53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" topLeftCell="H30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O53" sqref="O53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1444,56 +1444,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <v>1E-3</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8">
         <v>1E-4</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9">
+      <c r="E2" s="8"/>
+      <c r="F2" s="8">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9">
+      <c r="G2" s="8"/>
+      <c r="H2" s="8">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9">
+      <c r="I2" s="8"/>
+      <c r="J2" s="8">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9">
+      <c r="K2" s="8"/>
+      <c r="L2" s="8">
         <v>1E-8</v>
       </c>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9">
+      <c r="M2" s="8"/>
+      <c r="N2" s="8">
         <v>1.0000000000000001E-9</v>
       </c>
-      <c r="O2" s="9"/>
+      <c r="O2" s="8"/>
       <c r="P2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
@@ -1792,56 +1792,56 @@
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="8">
         <v>1E-3</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9">
+      <c r="C11" s="8"/>
+      <c r="D11" s="8">
         <v>1E-4</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9">
+      <c r="E11" s="8"/>
+      <c r="F11" s="8">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9">
+      <c r="G11" s="8"/>
+      <c r="H11" s="8">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9">
+      <c r="I11" s="8"/>
+      <c r="J11" s="8">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9">
+      <c r="K11" s="8"/>
+      <c r="L11" s="8">
         <v>1E-8</v>
       </c>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9">
+      <c r="M11" s="8"/>
+      <c r="N11" s="8">
         <v>1.0000000000000001E-9</v>
       </c>
-      <c r="O11" s="9"/>
+      <c r="O11" s="8"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -2126,56 +2126,56 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="8">
         <v>1E-3</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9">
+      <c r="C20" s="8"/>
+      <c r="D20" s="8">
         <v>1E-4</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9">
+      <c r="E20" s="8"/>
+      <c r="F20" s="8">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9">
+      <c r="G20" s="8"/>
+      <c r="H20" s="8">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9">
+      <c r="I20" s="8"/>
+      <c r="J20" s="8">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9">
+      <c r="K20" s="8"/>
+      <c r="L20" s="8">
         <v>1E-8</v>
       </c>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9">
+      <c r="M20" s="8"/>
+      <c r="N20" s="8">
         <v>1.0000000000000001E-9</v>
       </c>
-      <c r="O20" s="9"/>
+      <c r="O20" s="8"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
@@ -2460,56 +2460,56 @@
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="9">
+      <c r="B29" s="8">
         <v>1E-3</v>
       </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9">
+      <c r="C29" s="8"/>
+      <c r="D29" s="8">
         <v>1E-4</v>
       </c>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9">
+      <c r="E29" s="8"/>
+      <c r="F29" s="8">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9">
+      <c r="G29" s="8"/>
+      <c r="H29" s="8">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9">
+      <c r="I29" s="8"/>
+      <c r="J29" s="8">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9">
+      <c r="K29" s="8"/>
+      <c r="L29" s="8">
         <v>1E-8</v>
       </c>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9">
+      <c r="M29" s="8"/>
+      <c r="N29" s="8">
         <v>1.0000000000000001E-9</v>
       </c>
-      <c r="O29" s="9"/>
+      <c r="O29" s="8"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
@@ -2794,56 +2794,56 @@
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9"/>
+      <c r="N37" s="9"/>
+      <c r="O37" s="9"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B38" s="9">
+      <c r="B38" s="8">
         <v>1E-3</v>
       </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9">
+      <c r="C38" s="8"/>
+      <c r="D38" s="8">
         <v>1E-4</v>
       </c>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9">
+      <c r="E38" s="8"/>
+      <c r="F38" s="8">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9">
+      <c r="G38" s="8"/>
+      <c r="H38" s="8">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="I38" s="9"/>
-      <c r="J38" s="9">
+      <c r="I38" s="8"/>
+      <c r="J38" s="8">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="K38" s="9"/>
-      <c r="L38" s="9">
+      <c r="K38" s="8"/>
+      <c r="L38" s="8">
         <v>1E-8</v>
       </c>
-      <c r="M38" s="9"/>
-      <c r="N38" s="9">
+      <c r="M38" s="8"/>
+      <c r="N38" s="8">
         <v>1.0000000000000001E-9</v>
       </c>
-      <c r="O38" s="9"/>
+      <c r="O38" s="8"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
@@ -3128,56 +3128,56 @@
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A46" s="8" t="s">
+      <c r="A46" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
-      <c r="I46" s="8"/>
-      <c r="J46" s="8"/>
-      <c r="K46" s="8"/>
-      <c r="L46" s="8"/>
-      <c r="M46" s="8"/>
-      <c r="N46" s="8"/>
-      <c r="O46" s="8"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="9"/>
+      <c r="L46" s="9"/>
+      <c r="M46" s="9"/>
+      <c r="N46" s="9"/>
+      <c r="O46" s="9"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B47" s="9">
+      <c r="B47" s="8">
         <v>1E-3</v>
       </c>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9">
+      <c r="C47" s="8"/>
+      <c r="D47" s="8">
         <v>1E-4</v>
       </c>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9">
+      <c r="E47" s="8"/>
+      <c r="F47" s="8">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9">
+      <c r="G47" s="8"/>
+      <c r="H47" s="8">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="I47" s="9"/>
-      <c r="J47" s="9">
+      <c r="I47" s="8"/>
+      <c r="J47" s="8">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="K47" s="9"/>
-      <c r="L47" s="9">
+      <c r="K47" s="8"/>
+      <c r="L47" s="8">
         <v>1E-8</v>
       </c>
-      <c r="M47" s="9"/>
-      <c r="N47" s="9">
+      <c r="M47" s="8"/>
+      <c r="N47" s="8">
         <v>1.0000000000000001E-9</v>
       </c>
-      <c r="O47" s="9"/>
+      <c r="O47" s="8"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
@@ -3230,108 +3230,263 @@
       <c r="A49" s="2">
         <v>0.5</v>
       </c>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
-      <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
-      <c r="O49" s="2"/>
+      <c r="B49" s="2">
+        <v>7</v>
+      </c>
+      <c r="C49" s="2">
+        <v>6389942</v>
+      </c>
+      <c r="D49" s="2">
+        <v>10</v>
+      </c>
+      <c r="E49" s="2">
+        <v>8818346</v>
+      </c>
+      <c r="F49" s="2">
+        <v>13</v>
+      </c>
+      <c r="G49" s="2">
+        <v>11436280</v>
+      </c>
+      <c r="H49" s="2">
+        <v>16</v>
+      </c>
+      <c r="I49" s="2">
+        <v>14033506</v>
+      </c>
+      <c r="J49" s="2">
+        <v>19</v>
+      </c>
+      <c r="K49" s="2">
+        <v>16945143</v>
+      </c>
+      <c r="L49" s="2">
+        <v>22</v>
+      </c>
+      <c r="M49" s="2">
+        <v>20457355</v>
+      </c>
+      <c r="N49" s="2">
+        <v>25</v>
+      </c>
+      <c r="O49" s="2">
+        <v>21925912</v>
+      </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>0.7</v>
       </c>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
-      <c r="K50" s="2"/>
-      <c r="L50" s="2"/>
-      <c r="M50" s="2"/>
-      <c r="N50" s="2"/>
-      <c r="O50" s="2"/>
+      <c r="B50" s="2">
+        <v>12</v>
+      </c>
+      <c r="C50" s="2">
+        <v>10657564</v>
+      </c>
+      <c r="D50" s="2">
+        <v>17</v>
+      </c>
+      <c r="E50" s="2">
+        <v>16672719</v>
+      </c>
+      <c r="F50" s="2">
+        <v>23</v>
+      </c>
+      <c r="G50" s="2">
+        <v>20395170</v>
+      </c>
+      <c r="H50" s="2">
+        <v>29</v>
+      </c>
+      <c r="I50" s="2">
+        <v>25786252</v>
+      </c>
+      <c r="J50" s="2">
+        <v>36</v>
+      </c>
+      <c r="K50" s="2">
+        <v>32647767</v>
+      </c>
+      <c r="L50" s="2">
+        <v>42</v>
+      </c>
+      <c r="M50" s="2">
+        <v>36374790</v>
+      </c>
+      <c r="N50" s="2">
+        <v>48</v>
+      </c>
+      <c r="O50" s="2">
+        <v>41605552</v>
+      </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>0.85</v>
       </c>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
-      <c r="K51" s="2"/>
-      <c r="L51" s="2"/>
-      <c r="M51" s="2"/>
-      <c r="N51" s="2"/>
-      <c r="O51" s="2"/>
+      <c r="B51" s="2">
+        <v>23</v>
+      </c>
+      <c r="C51" s="2">
+        <v>19996063</v>
+      </c>
+      <c r="D51" s="2">
+        <v>35</v>
+      </c>
+      <c r="E51" s="2">
+        <v>30315705</v>
+      </c>
+      <c r="F51" s="2">
+        <v>48</v>
+      </c>
+      <c r="G51" s="2">
+        <v>41606010</v>
+      </c>
+      <c r="H51" s="2">
+        <v>61</v>
+      </c>
+      <c r="I51" s="2">
+        <v>52643154</v>
+      </c>
+      <c r="J51" s="2">
+        <v>74</v>
+      </c>
+      <c r="K51" s="2">
+        <v>64128632</v>
+      </c>
+      <c r="L51" s="2">
+        <v>88</v>
+      </c>
+      <c r="M51" s="2">
+        <v>81659969</v>
+      </c>
+      <c r="N51" s="2">
+        <v>102</v>
+      </c>
+      <c r="O51" s="2">
+        <v>87412849</v>
+      </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>0.9</v>
       </c>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
-      <c r="K52" s="2"/>
-      <c r="L52" s="2"/>
-      <c r="M52" s="2"/>
-      <c r="N52" s="2"/>
-      <c r="O52" s="2"/>
+      <c r="B52" s="2">
+        <v>32</v>
+      </c>
+      <c r="C52" s="2">
+        <v>27586440</v>
+      </c>
+      <c r="D52" s="2">
+        <v>51</v>
+      </c>
+      <c r="E52" s="2">
+        <v>43790240</v>
+      </c>
+      <c r="F52" s="2">
+        <v>71</v>
+      </c>
+      <c r="G52" s="2">
+        <v>60538652</v>
+      </c>
+      <c r="H52" s="2">
+        <v>92</v>
+      </c>
+      <c r="I52" s="2">
+        <v>78105307</v>
+      </c>
+      <c r="J52" s="2">
+        <v>112</v>
+      </c>
+      <c r="K52" s="2">
+        <v>95042430</v>
+      </c>
+      <c r="L52" s="2">
+        <v>133</v>
+      </c>
+      <c r="M52" s="2">
+        <v>112512266</v>
+      </c>
+      <c r="N52" s="2">
+        <v>154</v>
+      </c>
+      <c r="O52" s="2">
+        <v>129769915</v>
+      </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>0.99</v>
       </c>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
-      <c r="L53" s="2"/>
-      <c r="M53" s="2"/>
-      <c r="N53" s="2"/>
-      <c r="O53" s="2"/>
+      <c r="B53" s="2">
+        <v>222</v>
+      </c>
+      <c r="C53" s="2">
+        <v>193505360</v>
+      </c>
+      <c r="D53" s="2">
+        <v>428</v>
+      </c>
+      <c r="E53" s="2">
+        <v>381549444</v>
+      </c>
+      <c r="F53" s="2">
+        <v>647</v>
+      </c>
+      <c r="G53" s="2">
+        <v>543966523</v>
+      </c>
+      <c r="H53" s="2">
+        <v>871</v>
+      </c>
+      <c r="I53" s="2">
+        <v>730146694</v>
+      </c>
+      <c r="J53" s="2">
+        <v>1097</v>
+      </c>
+      <c r="K53" s="2">
+        <v>917326174</v>
+      </c>
+      <c r="L53" s="2">
+        <v>1324</v>
+      </c>
+      <c r="M53" s="2">
+        <v>1109483471</v>
+      </c>
+      <c r="N53" s="2">
+        <v>1551</v>
+      </c>
+      <c r="O53" s="2">
+        <v>1297167096</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A10:O10"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A46:O46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="L47:M47"/>
+    <mergeCell ref="N47:O47"/>
+    <mergeCell ref="A37:O37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="L38:M38"/>
+    <mergeCell ref="N38:O38"/>
+    <mergeCell ref="A28:O28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="N29:O29"/>
     <mergeCell ref="N11:O11"/>
     <mergeCell ref="A19:O19"/>
     <mergeCell ref="B20:C20"/>
@@ -3347,30 +3502,15 @@
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="L11:M11"/>
-    <mergeCell ref="A28:O28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="A37:O37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="L38:M38"/>
-    <mergeCell ref="N38:O38"/>
-    <mergeCell ref="A46:O46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="L47:M47"/>
-    <mergeCell ref="N47:O47"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A10:O10"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>